<commit_message>
added instructions in excelsheet
</commit_message>
<xml_diff>
--- a/AppFiles/Images/Logo/ConsumableBulkUpload.xlsx
+++ b/AppFiles/Images/Logo/ConsumableBulkUpload.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7110"/>
+    <workbookView windowWidth="19200" windowHeight="7110" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Asset ID</t>
   </si>
@@ -27,6 +28,18 @@
   <si>
     <t>Reorder Stock Quantity</t>
   </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>1. Asset ID should be a number.</t>
+  </si>
+  <si>
+    <t>2. Threshold Quantity should be a number.</t>
+  </si>
+  <si>
+    <t>3.Reorder Stock Quantity  should be a number.</t>
+  </si>
 </sst>
 </file>
 
@@ -35,8 +48,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -47,6 +60,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -54,23 +75,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -93,6 +107,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -115,21 +159,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -137,31 +166,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,23 +191,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,6 +221,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -219,175 +395,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,9 +441,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -451,11 +467,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,171 +512,162 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -969,8 +989,8 @@
   <sheetPr/>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
@@ -998,4 +1018,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="52.7272727272727" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="18.5" spans="1:1">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" ht="23" customHeight="1" spans="1:1">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="23" customHeight="1" spans="1:1">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="23" customHeight="1" spans="1:1">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>